<commit_message>
add requirement and file add delete
新增requeriement
edit 新增增加與刪除行
display 新增顏色
</commit_message>
<xml_diff>
--- a/competitions/test.xlsx
+++ b/competitions/test.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="21">
   <si>
     <t>比賽場序</t>
   </si>
@@ -52,16 +52,31 @@
     <t>大學男</t>
   </si>
   <si>
+    <t>大學南</t>
+  </si>
+  <si>
     <t>男一</t>
   </si>
   <si>
+    <t>南二</t>
+  </si>
+  <si>
+    <t>男三</t>
+  </si>
+  <si>
     <t>男二</t>
   </si>
   <si>
-    <t>男三</t>
+    <t>南寺</t>
   </si>
   <si>
     <t>男四</t>
+  </si>
+  <si>
+    <t>2.0</t>
+  </si>
+  <si>
+    <t>3.0</t>
   </si>
 </sst>
 </file>
@@ -453,16 +468,16 @@
         <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D2" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="E2" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="F2" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -473,10 +488,10 @@
         <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -484,10 +499,10 @@
         <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D4" t="s">
         <v>15</v>
@@ -498,13 +513,13 @@
         <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D5" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -515,10 +530,10 @@
         <v>11</v>
       </c>
       <c r="C6" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D6" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>